<commit_message>
Changes made as per comments from e5 team
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://quadance-my.sharepoint.com/personal/rahul_krishnan_quadance_com/Documents/UiPath/ACME/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{003C3A41-EB98-4A66-9412-1541DEED72D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{91BD3134-7AAF-4592-96FE-4A829719D06C}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{003C3A41-EB98-4A66-9412-1541DEED72D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2FCAAF3A-DE67-472D-89CC-2DE619F2330C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -80,6 +80,12 @@
   <si>
     <t>Receiver Mail ID</t>
   </si>
+  <si>
+    <t>ACME_Delay</t>
+  </si>
+  <si>
+    <t>Delay for Element Exist checks</t>
+  </si>
 </sst>
 </file>
 
@@ -130,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -142,6 +148,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2559,10 +2568,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2673,7 +2682,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="7">
+        <v>4000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3665,7 +3684,6 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>